<commit_message>
invoking server Service from Application.cfc
</commit_message>
<xml_diff>
--- a/temp/dataExcel.xlsx
+++ b/temp/dataExcel.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="76">
   <si>
     <t/>
   </si>
@@ -47,190 +47,199 @@
     <t>2024-10-23</t>
   </si>
   <si>
+    <t>2024-10-16 15:43:44.453</t>
+  </si>
+  <si>
+    <t>Cancelled</t>
+  </si>
+  <si>
+    <t>Dr. Rajesh Sharma</t>
+  </si>
+  <si>
+    <t>MBBS, MD</t>
+  </si>
+  <si>
+    <t>rajesh.sharma@example.com</t>
+  </si>
+  <si>
+    <t>Ayurveda</t>
+  </si>
+  <si>
+    <t>2024-10-24</t>
+  </si>
+  <si>
+    <t>2024-10-16 15:43:44.463</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Dr. Amit Verma</t>
+  </si>
+  <si>
+    <t>MBBS, DGO</t>
+  </si>
+  <si>
+    <t>amit.verma@example.com</t>
+  </si>
+  <si>
+    <t>Naturopathy</t>
+  </si>
+  <si>
+    <t>2024-10-25</t>
+  </si>
+  <si>
+    <t>2024-10-26</t>
+  </si>
+  <si>
+    <t>Dr. Anjali Meht</t>
+  </si>
+  <si>
+    <t>MBBS, MS</t>
+  </si>
+  <si>
+    <t>anjali.mehta@example.com</t>
+  </si>
+  <si>
+    <t>Yoga</t>
+  </si>
+  <si>
+    <t>2024-10-27</t>
+  </si>
+  <si>
+    <t>Dr. Ravi Kumar</t>
+  </si>
+  <si>
+    <t>MBBS, DCH</t>
+  </si>
+  <si>
+    <t>ravi.kumar@example.com</t>
+  </si>
+  <si>
+    <t>Homeopathy</t>
+  </si>
+  <si>
+    <t>2024-10-30</t>
+  </si>
+  <si>
+    <t>NoShow</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t>Dr. Priya Singh</t>
+  </si>
+  <si>
+    <t>MBBS, DDVL</t>
+  </si>
+  <si>
+    <t>priya.singh@example.com</t>
+  </si>
+  <si>
+    <t>Allopathy</t>
+  </si>
+  <si>
+    <t>2024-11-05</t>
+  </si>
+  <si>
+    <t>2024-11-05 10:48:23.673</t>
+  </si>
+  <si>
+    <t>Dr. Neha Gupta</t>
+  </si>
+  <si>
+    <t>neha.gupta@example.com</t>
+  </si>
+  <si>
+    <t>2024-11-05 10:48:36.99</t>
+  </si>
+  <si>
+    <t>2024-11-13</t>
+  </si>
+  <si>
+    <t>2024-11-12 15:25:34.6</t>
+  </si>
+  <si>
+    <t>2024-11-14</t>
+  </si>
+  <si>
+    <t>2024-11-13 17:51:55.68</t>
+  </si>
+  <si>
+    <t>Dr. Karan Singh</t>
+  </si>
+  <si>
+    <t>MBBS, DNB</t>
+  </si>
+  <si>
+    <t>karan.singh@example.com</t>
+  </si>
+  <si>
+    <t>2024-11-14 12:48:57.417</t>
+  </si>
+  <si>
+    <t>2024-11-14 12:49:29.223</t>
+  </si>
+  <si>
+    <t>2024-11-14 12:50:06.84</t>
+  </si>
+  <si>
+    <t>2024-11-14 12:52:41.9</t>
+  </si>
+  <si>
+    <t>2024-11-15</t>
+  </si>
+  <si>
+    <t>2024-11-15 09:57:07.37</t>
+  </si>
+  <si>
+    <t>2024-11-15 11:04:29.11</t>
+  </si>
+  <si>
+    <t>2024-11-15 15:24:57.52</t>
+  </si>
+  <si>
+    <t>Confirmed</t>
+  </si>
+  <si>
+    <t>2024-11-16</t>
+  </si>
+  <si>
+    <t>2024-11-15 17:37:01.24</t>
+  </si>
+  <si>
+    <t>2024-11-18</t>
+  </si>
+  <si>
+    <t>2024-11-18 10:22:38.827</t>
+  </si>
+  <si>
+    <t>2024-11-18 10:23:29.15</t>
+  </si>
+  <si>
+    <t>2024-11-18 15:23:13.84</t>
+  </si>
+  <si>
+    <t>2024-11-18 15:45:49.663</t>
+  </si>
+  <si>
+    <t>2024-11-19</t>
+  </si>
+  <si>
+    <t>2024-11-18 16:49:31.233</t>
+  </si>
+  <si>
+    <t>2024-11-20</t>
+  </si>
+  <si>
+    <t>2024-11-18 17:38:40.683</t>
+  </si>
+  <si>
+    <t>2024-11-21</t>
+  </si>
+  <si>
     <t>2024-10-22 14:28:35.923</t>
-  </si>
-  <si>
-    <t>NoShow</t>
-  </si>
-  <si>
-    <t>Dr. Neha Gupta</t>
-  </si>
-  <si>
-    <t>MBBS, MD</t>
-  </si>
-  <si>
-    <t>neha.gupta@example.com</t>
-  </si>
-  <si>
-    <t>Ayurveda</t>
-  </si>
-  <si>
-    <t>2024-10-16 15:43:44.453</t>
-  </si>
-  <si>
-    <t>Cancelled</t>
-  </si>
-  <si>
-    <t>Dr. Rajesh Sharma</t>
-  </si>
-  <si>
-    <t>rajesh.sharma@example.com</t>
-  </si>
-  <si>
-    <t>2024-10-24</t>
-  </si>
-  <si>
-    <t>2024-10-16 15:43:44.463</t>
-  </si>
-  <si>
-    <t>Completed</t>
-  </si>
-  <si>
-    <t>Dr. Amit Verma</t>
-  </si>
-  <si>
-    <t>MBBS, DGO</t>
-  </si>
-  <si>
-    <t>amit.verma@example.com</t>
-  </si>
-  <si>
-    <t>Naturopathy</t>
-  </si>
-  <si>
-    <t>2024-10-25</t>
-  </si>
-  <si>
-    <t>2024-10-26</t>
-  </si>
-  <si>
-    <t>Dr. Anjali Meht</t>
-  </si>
-  <si>
-    <t>MBBS, MS</t>
-  </si>
-  <si>
-    <t>anjali.mehta@example.com</t>
-  </si>
-  <si>
-    <t>Yoga</t>
-  </si>
-  <si>
-    <t>2024-10-27</t>
-  </si>
-  <si>
-    <t>Dr. Ravi Kumar</t>
-  </si>
-  <si>
-    <t>MBBS, DCH</t>
-  </si>
-  <si>
-    <t>ravi.kumar@example.com</t>
-  </si>
-  <si>
-    <t>Homeopathy</t>
-  </si>
-  <si>
-    <t>2024-10-30</t>
-  </si>
-  <si>
-    <t>Pending</t>
-  </si>
-  <si>
-    <t>Dr. Priya Singh</t>
-  </si>
-  <si>
-    <t>MBBS, DDVL</t>
-  </si>
-  <si>
-    <t>priya.singh@example.com</t>
-  </si>
-  <si>
-    <t>Allopathy</t>
-  </si>
-  <si>
-    <t>2024-11-05</t>
-  </si>
-  <si>
-    <t>2024-11-05 10:48:23.673</t>
-  </si>
-  <si>
-    <t>2024-11-05 10:48:36.99</t>
-  </si>
-  <si>
-    <t>2024-11-13</t>
-  </si>
-  <si>
-    <t>2024-11-12 15:25:34.6</t>
-  </si>
-  <si>
-    <t>2024-11-14</t>
-  </si>
-  <si>
-    <t>2024-11-13 17:51:55.68</t>
-  </si>
-  <si>
-    <t>Dr. Karan Singh</t>
-  </si>
-  <si>
-    <t>MBBS, DNB</t>
-  </si>
-  <si>
-    <t>karan.singh@example.com</t>
-  </si>
-  <si>
-    <t>2024-11-14 12:48:57.417</t>
-  </si>
-  <si>
-    <t>2024-11-14 12:49:29.223</t>
-  </si>
-  <si>
-    <t>2024-11-14 12:50:06.84</t>
-  </si>
-  <si>
-    <t>2024-11-14 12:52:41.9</t>
-  </si>
-  <si>
-    <t>2024-11-15</t>
-  </si>
-  <si>
-    <t>2024-11-15 09:57:07.37</t>
-  </si>
-  <si>
-    <t>2024-11-15 11:04:29.11</t>
-  </si>
-  <si>
-    <t>2024-11-15 15:24:57.52</t>
-  </si>
-  <si>
-    <t>2024-11-16</t>
-  </si>
-  <si>
-    <t>2024-11-15 17:37:01.24</t>
-  </si>
-  <si>
-    <t>2024-11-18</t>
-  </si>
-  <si>
-    <t>2024-11-18 10:22:38.827</t>
-  </si>
-  <si>
-    <t>Confirmed</t>
-  </si>
-  <si>
-    <t>2024-11-18 10:23:29.15</t>
-  </si>
-  <si>
-    <t>2024-11-18 15:23:13.84</t>
-  </si>
-  <si>
-    <t>2024-11-18 15:45:49.663</t>
-  </si>
-  <si>
-    <t>2024-11-19</t>
-  </si>
-  <si>
-    <t>2024-11-18 16:49:31.233</t>
   </si>
 </sst>
 </file>
@@ -279,7 +288,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -327,7 +336,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>11.0</v>
+        <v>1.0</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -348,7 +357,7 @@
         <v>15</v>
       </c>
       <c r="H2" t="n">
-        <v>9.988775544E9</v>
+        <v>9.87654321E9</v>
       </c>
       <c r="I2" t="s">
         <v>16</v>
@@ -356,257 +365,257 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H3" t="n">
-        <v>9.87654321E9</v>
+        <v>9.7654321E9</v>
       </c>
       <c r="I3" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="G4" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="H4" t="n">
-        <v>9.7654321E9</v>
+        <v>9.87654321E9</v>
       </c>
       <c r="I4" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" t="s">
         <v>28</v>
       </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" t="s">
-        <v>20</v>
-      </c>
       <c r="H5" t="n">
-        <v>9.87654321E9</v>
+        <v>9.12345678E9</v>
       </c>
       <c r="I5" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H6" t="n">
-        <v>9.12345678E9</v>
+        <v>9.988776655E9</v>
       </c>
       <c r="I6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>8.0</v>
+        <v>2.0</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="F7" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="G7" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="H7" t="n">
-        <v>9.988776655E9</v>
+        <v>9.12345678E9</v>
       </c>
       <c r="I7" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="E8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H8" t="n">
-        <v>9.12345678E9</v>
+        <v>9.988776655E9</v>
       </c>
       <c r="I8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" t="s">
         <v>39</v>
       </c>
-      <c r="C9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="G9" t="s">
         <v>40</v>
       </c>
-      <c r="E9" t="s">
-        <v>35</v>
-      </c>
-      <c r="F9" t="s">
-        <v>36</v>
-      </c>
-      <c r="G9" t="s">
-        <v>37</v>
-      </c>
       <c r="H9" t="n">
-        <v>9.988776655E9</v>
+        <v>9.871234567E9</v>
       </c>
       <c r="I9" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>4.0</v>
+        <v>21.0</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="E10" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F10" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="G10" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="H10" t="n">
-        <v>9.871234567E9</v>
+        <v>9.988775544E9</v>
       </c>
       <c r="I10" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>21.0</v>
+        <v>22.0</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
         <v>46</v>
       </c>
       <c r="D11" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="E11" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="F11" t="s">
         <v>14</v>
       </c>
       <c r="G11" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="H11" t="n">
         <v>9.988775544E9</v>
@@ -617,25 +626,25 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>22.0</v>
+        <v>25.0</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D12" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="E12" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="F12" t="s">
         <v>14</v>
       </c>
       <c r="G12" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="H12" t="n">
         <v>9.988775544E9</v>
@@ -646,326 +655,326 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>25.0</v>
+        <v>26.0</v>
       </c>
       <c r="B13" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D13" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="E13" t="s">
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="F13" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="G13" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="H13" t="n">
-        <v>9.988775544E9</v>
+        <v>9.876543234E9</v>
       </c>
       <c r="I13" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>26.0</v>
+        <v>31.0</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D14" t="s">
         <v>12</v>
       </c>
       <c r="E14" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="F14" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="G14" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="H14" t="n">
-        <v>9.876543234E9</v>
+        <v>9.12345678E9</v>
       </c>
       <c r="I14" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>31.0</v>
+        <v>32.0</v>
       </c>
       <c r="B15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C15" t="s">
         <v>55</v>
       </c>
       <c r="D15" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="E15" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F15" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G15" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H15" t="n">
         <v>9.12345678E9</v>
       </c>
       <c r="I15" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>32.0</v>
+        <v>33.0</v>
       </c>
       <c r="B16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C16" t="s">
         <v>56</v>
       </c>
       <c r="D16" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E16" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="F16" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="G16" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="H16" t="n">
-        <v>9.12345678E9</v>
+        <v>9.876543234E9</v>
       </c>
       <c r="I16" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>33.0</v>
+        <v>34.0</v>
       </c>
       <c r="B17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C17" t="s">
         <v>57</v>
       </c>
       <c r="D17" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="E17" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="F17" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="G17" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="H17" t="n">
-        <v>9.876543234E9</v>
+        <v>9.988776655E9</v>
       </c>
       <c r="I17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>34.0</v>
+        <v>35.0</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="C18" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D18" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E18" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="F18" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="G18" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="H18" t="n">
-        <v>9.988776655E9</v>
+        <v>9.988775544E9</v>
       </c>
       <c r="I18" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>35.0</v>
+        <v>36.0</v>
       </c>
       <c r="B19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C19" t="s">
         <v>60</v>
       </c>
       <c r="D19" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="E19" t="s">
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="F19" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="G19" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="H19" t="n">
-        <v>9.988775544E9</v>
+        <v>9.876543234E9</v>
       </c>
       <c r="I19" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>36.0</v>
+        <v>42.0</v>
       </c>
       <c r="B20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C20" t="s">
         <v>61</v>
       </c>
       <c r="D20" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="E20" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="F20" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="G20" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="H20" t="n">
-        <v>9.876543234E9</v>
+        <v>9.988776655E9</v>
       </c>
       <c r="I20" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>42.0</v>
+        <v>43.0</v>
       </c>
       <c r="B21" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C21" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D21" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="E21" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="F21" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="G21" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="H21" t="n">
-        <v>9.988776655E9</v>
+        <v>9.12345678E9</v>
       </c>
       <c r="I21" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>43.0</v>
+        <v>44.0</v>
       </c>
       <c r="B22" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C22" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D22" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="E22" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F22" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G22" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H22" t="n">
         <v>9.12345678E9</v>
       </c>
       <c r="I22" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>44.0</v>
+        <v>45.0</v>
       </c>
       <c r="B23" t="s">
         <v>65</v>
       </c>
       <c r="C23" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D23" t="s">
-        <v>67</v>
+        <v>12</v>
       </c>
       <c r="E23" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F23" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G23" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H23" t="n">
-        <v>9.12345678E9</v>
+        <v>9.988776655E9</v>
       </c>
       <c r="I23" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>45.0</v>
+        <v>46.0</v>
       </c>
       <c r="B24" t="s">
         <v>65</v>
@@ -974,27 +983,27 @@
         <v>68</v>
       </c>
       <c r="D24" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E24" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F24" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G24" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="H24" t="n">
         <v>9.988776655E9</v>
       </c>
       <c r="I24" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>46.0</v>
+        <v>47.0</v>
       </c>
       <c r="B25" t="s">
         <v>65</v>
@@ -1003,79 +1012,108 @@
         <v>69</v>
       </c>
       <c r="D25" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E25" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F25" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="G25" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="H25" t="n">
-        <v>9.988776655E9</v>
+        <v>9.871234567E9</v>
       </c>
       <c r="I25" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>47.0</v>
+        <v>48.0</v>
       </c>
       <c r="B26" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="C26" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D26" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E26" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F26" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="G26" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="H26" t="n">
-        <v>9.871234567E9</v>
+        <v>9.988775544E9</v>
       </c>
       <c r="I26" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>48.0</v>
+        <v>49.0</v>
       </c>
       <c r="B27" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C27" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D27" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="E27" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="F27" t="s">
+        <v>32</v>
+      </c>
+      <c r="G27" t="s">
+        <v>33</v>
+      </c>
+      <c r="H27" t="n">
+        <v>9.988776655E9</v>
+      </c>
+      <c r="I27" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="B28" t="s">
+        <v>74</v>
+      </c>
+      <c r="C28" t="s">
+        <v>75</v>
+      </c>
+      <c r="D28" t="s">
+        <v>37</v>
+      </c>
+      <c r="E28" t="s">
+        <v>44</v>
+      </c>
+      <c r="F28" t="s">
         <v>14</v>
       </c>
-      <c r="G27" t="s">
-        <v>15</v>
-      </c>
-      <c r="H27" t="n">
+      <c r="G28" t="s">
+        <v>45</v>
+      </c>
+      <c r="H28" t="n">
         <v>9.988775544E9</v>
       </c>
-      <c r="I27" t="s">
+      <c r="I28" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>